<commit_message>
Method to take Email sender from cripted data in txt file
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
   <si>
     <t>name</t>
   </si>
@@ -33,16 +33,70 @@
     <t>attachments</t>
   </si>
   <si>
-    <t xml:space="preserve">اسلام </t>
+    <t>الاستاذ</t>
+  </si>
+  <si>
+    <t>file2.txt,file3.txt</t>
   </si>
   <si>
     <t>no5510425@gmail.com</t>
   </si>
   <si>
-    <t>file1.txt</t>
-  </si>
-  <si>
-    <t>الاستاذ</t>
+    <t>Job-title</t>
+  </si>
+  <si>
+    <t>مهندس</t>
+  </si>
+  <si>
+    <t>file name</t>
+  </si>
+  <si>
+    <t>إبراهيم عبدالعزيز</t>
+  </si>
+  <si>
+    <t>Ibrahim-Abdel-Aziz</t>
+  </si>
+  <si>
+    <t>عاطف العباسي</t>
+  </si>
+  <si>
+    <t>atif.alabbasi@gmail.com</t>
+  </si>
+  <si>
+    <t>الاستاااااذ</t>
+  </si>
+  <si>
+    <t>إدارة الحلول المتكاملة</t>
+  </si>
+  <si>
+    <t>crt_Part_1.pdf</t>
+  </si>
+  <si>
+    <t>Abbasi's-affection</t>
+  </si>
+  <si>
+    <t>ATIF ALABBASI</t>
+  </si>
+  <si>
+    <t>dev@una-oic.org</t>
+  </si>
+  <si>
+    <t>Engineer</t>
+  </si>
+  <si>
+    <t>Telecommunications</t>
+  </si>
+  <si>
+    <t>وسيل العلوي</t>
+  </si>
+  <si>
+    <t>الأستاذة</t>
+  </si>
+  <si>
+    <t>الإدارة القانونية</t>
+  </si>
+  <si>
+    <t>wasil-alealwi</t>
   </si>
 </sst>
 </file>
@@ -58,12 +112,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
+      <color theme="1"/>
+      <name val="Tahoma"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -83,16 +135,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -100,6 +152,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -392,55 +447,132 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="25.42578125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="4" width="25.42578125" style="1"/>
+    <col min="5" max="5" width="7" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="25.42578125" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="1">
+        <v>3</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
+      <c r="G3" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="1"/>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="1">
+        <v>5</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="1">
+        <v>9</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="1">
+        <v>15</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
update From_email Gmail sebder
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27830"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F599F7E1-D254-4860-A91C-3B9FDC2ADDBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>name</t>
   </si>
@@ -30,79 +31,22 @@
     <t>id</t>
   </si>
   <si>
-    <t>attachments</t>
-  </si>
-  <si>
     <t>الاستاذ</t>
   </si>
   <si>
-    <t>file2.txt,file3.txt</t>
+    <t>noone5510425@outlook.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">اسلام </t>
   </si>
   <si>
     <t>no5510425@gmail.com</t>
-  </si>
-  <si>
-    <t>Job-title</t>
-  </si>
-  <si>
-    <t>مهندس</t>
-  </si>
-  <si>
-    <t>file name</t>
-  </si>
-  <si>
-    <t>إبراهيم عبدالعزيز</t>
-  </si>
-  <si>
-    <t>Ibrahim-Abdel-Aziz</t>
-  </si>
-  <si>
-    <t>عاطف العباسي</t>
-  </si>
-  <si>
-    <t>atif.alabbasi@gmail.com</t>
-  </si>
-  <si>
-    <t>الاستاااااذ</t>
-  </si>
-  <si>
-    <t>إدارة الحلول المتكاملة</t>
-  </si>
-  <si>
-    <t>crt_Part_1.pdf</t>
-  </si>
-  <si>
-    <t>Abbasi's-affection</t>
-  </si>
-  <si>
-    <t>ATIF ALABBASI</t>
-  </si>
-  <si>
-    <t>dev@una-oic.org</t>
-  </si>
-  <si>
-    <t>Engineer</t>
-  </si>
-  <si>
-    <t>Telecommunications</t>
-  </si>
-  <si>
-    <t>وسيل العلوي</t>
-  </si>
-  <si>
-    <t>الأستاذة</t>
-  </si>
-  <si>
-    <t>الإدارة القانونية</t>
-  </si>
-  <si>
-    <t>wasil-alealwi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -112,10 +56,12 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Tahoma"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -135,16 +81,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -161,9 +107,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -201,7 +147,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -273,7 +219,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -446,139 +392,361 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:G5"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="25.42578125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="4" width="25.42578125" style="1"/>
-    <col min="5" max="5" width="7" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="25.42578125" style="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="1">
-        <v>3</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="1">
-        <v>5</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="1">
-        <v>9</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="1">
-        <v>15</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>26</v>
-      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="1"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="1"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="1"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="1"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="1"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="1"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="1"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="1"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="1"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B23" s="1"/>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B24" s="1"/>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B25" s="1"/>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B26" s="1"/>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B27" s="1"/>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B28" s="1"/>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B29" s="1"/>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B30" s="1"/>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B31" s="1"/>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B32" s="1"/>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" s="1"/>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" s="1"/>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35" s="1"/>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B36" s="1"/>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B37" s="1"/>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B38" s="1"/>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B39" s="1"/>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B40" s="1"/>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B41" s="1"/>
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B42" s="1"/>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B43" s="1"/>
+    </row>
+    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B44" s="1"/>
+    </row>
+    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B45" s="1"/>
+    </row>
+    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B46" s="1"/>
+    </row>
+    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B47" s="1"/>
+    </row>
+    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B48" s="1"/>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B49" s="1"/>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B50" s="1"/>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B51" s="1"/>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B52" s="1"/>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B53" s="1"/>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B54" s="1"/>
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B55" s="1"/>
+    </row>
+    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B56" s="1"/>
+    </row>
+    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B57" s="1"/>
+    </row>
+    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B58" s="1"/>
+    </row>
+    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B59" s="1"/>
+    </row>
+    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B60" s="1"/>
+    </row>
+    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B61" s="1"/>
+    </row>
+    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B62" s="1"/>
+    </row>
+    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B63" s="1"/>
+    </row>
+    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B64" s="1"/>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B65" s="1"/>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B66" s="1"/>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B67" s="1"/>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B68" s="1"/>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B69" s="1"/>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B70" s="1"/>
+    </row>
+    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B71" s="1"/>
+    </row>
+    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B72" s="1"/>
+    </row>
+    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B73" s="1"/>
+    </row>
+    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B74" s="1"/>
+    </row>
+    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B75" s="1"/>
+    </row>
+    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B76" s="1"/>
+    </row>
+    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B77" s="1"/>
+    </row>
+    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B78" s="1"/>
+    </row>
+    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B79" s="1"/>
+    </row>
+    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B80" s="1"/>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B81" s="1"/>
+    </row>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B82" s="1"/>
+    </row>
+    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B83" s="1"/>
+    </row>
+    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B84" s="1"/>
+    </row>
+    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B85" s="1"/>
+    </row>
+    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B86" s="1"/>
+    </row>
+    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B87" s="1"/>
+    </row>
+    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B88" s="1"/>
+    </row>
+    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B89" s="1"/>
+    </row>
+    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B90" s="1"/>
+    </row>
+    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B91" s="1"/>
+    </row>
+    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B92" s="1"/>
+    </row>
+    <row r="93" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B93" s="1"/>
+    </row>
+    <row r="94" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B94" s="1"/>
+    </row>
+    <row r="95" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B95" s="1"/>
+    </row>
+    <row r="96" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B96" s="1"/>
+    </row>
+    <row r="97" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B97" s="1"/>
+    </row>
+    <row r="98" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B98" s="1"/>
+    </row>
+    <row r="99" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B99" s="1"/>
+    </row>
+    <row r="100" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B100" s="1"/>
+    </row>
+    <row r="101" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B101" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{9B1BD282-98B4-4097-AEBC-AD19CF67A242}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -590,7 +758,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>